<commit_message>
service-provider seed data modified
</commit_message>
<xml_diff>
--- a/service-provider-profile-service/src/main/resources/Seed_Ideas2.xlsx
+++ b/service-provider-profile-service/src/main/resources/Seed_Ideas2.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="163">
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="162">
   <si>
     <t xml:space="preserve">MAIL ID</t>
   </si>
@@ -605,7 +602,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -616,10 +613,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -715,26 +708,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="82.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="37.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="37.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="82.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="37.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="11" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -762,18 +755,15 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -797,18 +787,15 @@
       <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="4" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="5" t="n">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -832,28 +819,25 @@
       <c r="I3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="4" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="5" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>32</v>
@@ -867,31 +851,28 @@
       <c r="I4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="4" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="5" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>40</v>
@@ -902,28 +883,25 @@
       <c r="I5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="4" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="5" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>47</v>
@@ -937,28 +915,25 @@
       <c r="I6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="4" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K6" s="5" t="n">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>55</v>
@@ -966,57 +941,51 @@
       <c r="G7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="4" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="5" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="1" t="s">
         <v>65</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="4" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="K8" s="5" t="n">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
-        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>68</v>
@@ -1025,16 +994,16 @@
         <v>69</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>72</v>
@@ -1042,16 +1011,13 @@
       <c r="I9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="6" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="K9" s="7" t="n">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
-        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>75</v>
@@ -1060,10 +1026,10 @@
         <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>78</v>
@@ -1077,16 +1043,13 @@
       <c r="I10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="6" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="K10" s="7" t="n">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
-        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>83</v>
@@ -1095,16 +1058,16 @@
         <v>84</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>87</v>
@@ -1112,16 +1075,13 @@
       <c r="I11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="6" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="K11" s="7" t="n">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
-        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>90</v>
@@ -1130,10 +1090,10 @@
         <v>91</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>93</v>
@@ -1147,16 +1107,13 @@
       <c r="I12" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="6" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="K12" s="7" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
-        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>98</v>
@@ -1165,16 +1122,16 @@
         <v>99</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>102</v>
@@ -1182,16 +1139,13 @@
       <c r="I13" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="6" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="K13" s="7" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
-        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>105</v>
@@ -1200,10 +1154,10 @@
         <v>106</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>108</v>
@@ -1217,16 +1171,13 @@
       <c r="I14" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="6" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="K14" s="7" t="n">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
-        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>113</v>
@@ -1252,16 +1203,13 @@
       <c r="I15" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="6" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="K15" s="7" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
-        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>122</v>
@@ -1270,10 +1218,10 @@
         <v>123</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>125</v>
@@ -1287,31 +1235,28 @@
       <c r="I16" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="6" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="K16" s="7" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>131</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>133</v>
@@ -1322,28 +1267,25 @@
       <c r="I17" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="6" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="K17" s="7" t="n">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="1" t="s">
         <v>137</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>138</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>140</v>
@@ -1357,16 +1299,13 @@
       <c r="I18" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="6" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="K18" s="7" t="n">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
-        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>145</v>
@@ -1375,16 +1314,16 @@
         <v>146</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>147</v>
+        <v>13</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>33</v>
+        <v>147</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>148</v>
@@ -1392,16 +1331,13 @@
       <c r="I19" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="6" t="n">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="K19" s="7" t="n">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
-        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>151</v>
@@ -1410,16 +1346,16 @@
         <v>152</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>154</v>
@@ -1427,16 +1363,13 @@
       <c r="I20" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="6" t="n">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="K20" s="7" t="n">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
-        <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>157</v>
@@ -1445,16 +1378,16 @@
         <v>158</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>159</v>
+        <v>13</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>40</v>
+        <v>159</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>160</v>
@@ -1462,25 +1395,22 @@
       <c r="I21" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="K21" s="7" t="n">
+      <c r="J21" s="6" t="n">
         <v>1000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="shebymbabu@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId2" display="ryansujith@gmail.com"/>
-    <hyperlink ref="B4" r:id="rId3" display="elwin@yahoo.com"/>
-    <hyperlink ref="B5" r:id="rId4" display="maya@gmail.com"/>
-    <hyperlink ref="B6" r:id="rId5" display="ashokkumar@gmail.cm"/>
-    <hyperlink ref="B7" r:id="rId6" display="jui@gmail.com"/>
-    <hyperlink ref="B8" r:id="rId7" display="shetty@gmail.com"/>
-    <hyperlink ref="C8" r:id="rId8" display="Shetty@1234"/>
-    <hyperlink ref="B17" r:id="rId9" display="yashaswindtz2gmail.com"/>
-    <hyperlink ref="B18" r:id="rId10" display="mayank2gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="shebymbabu@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="ryansujith@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId3" display="elwin@yahoo.com"/>
+    <hyperlink ref="A5" r:id="rId4" display="maya@gmail.com"/>
+    <hyperlink ref="A6" r:id="rId5" display="ashokkumar@gmail.cm"/>
+    <hyperlink ref="A7" r:id="rId6" display="jui@gmail.com"/>
+    <hyperlink ref="A8" r:id="rId7" display="shetty@gmail.com"/>
+    <hyperlink ref="B8" r:id="rId8" display="Shetty@1234"/>
+    <hyperlink ref="A17" r:id="rId9" display="yashaswindtz2gmail.com"/>
+    <hyperlink ref="A18" r:id="rId10" display="mayank2gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
changes in service-provider xlsx file
</commit_message>
<xml_diff>
--- a/service-provider-profile-service/src/main/resources/Seed_Ideas2.xlsx
+++ b/service-provider-profile-service/src/main/resources/Seed_Ideas2.xlsx
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Maya</t>
   </si>
   <si>
-    <t xml:space="preserve">Web developer</t>
+    <t xml:space="preserve">Web Developer</t>
   </si>
   <si>
     <t xml:space="preserve">HTML, Bootstrap, PHP</t>
@@ -711,7 +711,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>